<commit_message>
Use logged output variable
Updates to perform analysis only on logged output variable
</commit_message>
<xml_diff>
--- a/Input/Rope Data.xlsx
+++ b/Input/Rope Data.xlsx
@@ -42,10 +42,10 @@
     <t>Order Within Block</t>
   </si>
   <si>
-    <t>Additional Length with Weight (In Inches)</t>
+    <t>Polypropylene</t>
   </si>
   <si>
-    <t>Polypropylene</t>
+    <t>Additional Length with Weight Inches</t>
   </si>
 </sst>
 </file>
@@ -556,7 +556,7 @@
   <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B17"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -578,7 +578,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
         <v>6</v>
@@ -589,7 +589,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1">
         <v>0.5</v>
@@ -606,7 +606,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1">
         <v>0.25</v>
@@ -623,7 +623,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1">
         <v>0.625</v>
@@ -640,7 +640,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1">
         <v>0.25</v>
@@ -657,7 +657,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1">
         <v>0.5</v>
@@ -675,7 +675,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1">
         <v>0.375</v>
@@ -693,7 +693,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1">
         <v>0.625</v>
@@ -711,7 +711,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1">
         <v>0.375</v>
@@ -729,7 +729,7 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1">
         <v>0.625</v>
@@ -746,7 +746,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="1">
         <v>0.25</v>
@@ -764,7 +764,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="1">
         <v>0.5</v>
@@ -781,7 +781,7 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="1">
         <v>0.25</v>
@@ -799,7 +799,7 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="1">
         <v>0.625</v>
@@ -816,7 +816,7 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" s="1">
         <v>0.375</v>
@@ -834,7 +834,7 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16" s="1">
         <v>0.5</v>
@@ -852,7 +852,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" s="1">
         <v>0.375</v>

</xml_diff>